<commit_message>
FilterScreens united, Allure steps added. Some cleaning
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Netology\QA-Finale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71765B84-F518-48A8-B348-479F141F2AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35F5AD1-16A1-44E3-A005-E5F4E2C1E290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8970" yWindow="1200" windowWidth="23580" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="152">
   <si>
     <t>Экран загрузки</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>Меню пользователя</t>
+  </si>
+  <si>
+    <t>Покрытие автотестами</t>
+  </si>
+  <si>
+    <t>Не покрыт. Нет фильтрации заявок из главного окна. Работает из окна заявок</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -624,6 +630,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -906,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,10 +936,11 @@
     <col min="5" max="5" width="41.140625" style="8" customWidth="1"/>
     <col min="6" max="6" width="47" style="8" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="5"/>
+    <col min="8" max="8" width="20" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="97.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
@@ -946,8 +962,11 @@
       <c r="G1" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -967,12 +986,15 @@
       <c r="G2" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H2" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -990,12 +1012,15 @@
       <c r="G3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="H3" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
         <v>42</v>
       </c>
@@ -1011,12 +1036,15 @@
       <c r="G4" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H4" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
         <v>43</v>
       </c>
@@ -1032,12 +1060,15 @@
       <c r="G5" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H5" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1055,12 +1086,15 @@
       <c r="G6" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="9"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1076,12 +1110,15 @@
       <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H7" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="9"/>
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
         <v>65</v>
       </c>
@@ -1097,12 +1134,15 @@
       <c r="G8" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H8" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="9"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
@@ -1118,12 +1158,15 @@
       <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H9" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1139,12 +1182,15 @@
       <c r="G10" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1160,12 +1206,15 @@
       <c r="G11" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1181,12 +1230,15 @@
       <c r="G12" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H12" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1202,12 +1254,15 @@
       <c r="G13" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1225,12 +1280,15 @@
       <c r="G14" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H14" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1246,12 +1304,15 @@
       <c r="G15" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="9"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1267,12 +1328,15 @@
       <c r="G16" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H16" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="9"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
@@ -1288,12 +1352,15 @@
       <c r="G17" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H17" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
@@ -1309,12 +1376,15 @@
       <c r="G18" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H18" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="9"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1330,12 +1400,13 @@
       <c r="G19" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="9"/>
+      <c r="B20" s="10"/>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
@@ -1351,12 +1422,13 @@
       <c r="G20" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="9"/>
+      <c r="B21" s="10"/>
       <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
@@ -1372,12 +1444,15 @@
       <c r="G21" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H21" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="9"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
@@ -1393,12 +1468,13 @@
       <c r="G22" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="9"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="1" t="s">
         <v>18</v>
       </c>
@@ -1414,12 +1490,13 @@
       <c r="G23" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="10"/>
       <c r="C24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1435,12 +1512,13 @@
       <c r="G24" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H24" s="11"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="9"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1456,12 +1534,15 @@
       <c r="G25" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H25" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="9"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="1" t="s">
         <v>20</v>
       </c>
@@ -1477,12 +1558,15 @@
       <c r="G26" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H26" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="9"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1498,12 +1582,15 @@
       <c r="G27" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H27" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1521,12 +1608,15 @@
       <c r="G28" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H28" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1542,12 +1632,15 @@
       <c r="G29" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H29" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1563,12 +1656,15 @@
       <c r="G30" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H30" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="10"/>
       <c r="C31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1584,12 +1680,15 @@
       <c r="G31" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H31" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1607,12 +1706,15 @@
       <c r="G32" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H32" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="1" t="s">
         <v>29</v>
       </c>
@@ -1628,12 +1730,15 @@
       <c r="G33" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H33" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="10"/>
       <c r="C34" s="1" t="s">
         <v>127</v>
       </c>
@@ -1649,12 +1754,15 @@
       <c r="G34" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H34" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1670,12 +1778,15 @@
       <c r="G35" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H35" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="1" t="s">
         <v>132</v>
       </c>
@@ -1691,12 +1802,15 @@
       <c r="G36" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H36" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="1" t="s">
         <v>31</v>
       </c>
@@ -1712,12 +1826,15 @@
       <c r="G37" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H37" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>37</v>
       </c>
-      <c r="B38" s="9"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1733,12 +1850,15 @@
       <c r="G38" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H38" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>38</v>
       </c>
-      <c r="B39" s="9"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
@@ -1754,12 +1874,15 @@
       <c r="G39" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H39" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
-      <c r="B40" s="9"/>
+      <c r="B40" s="10"/>
       <c r="C40" s="1" t="s">
         <v>138</v>
       </c>
@@ -1775,12 +1898,15 @@
       <c r="G40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H40" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40</v>
       </c>
-      <c r="B41" s="9"/>
+      <c r="B41" s="10"/>
       <c r="C41" s="1" t="s">
         <v>34</v>
       </c>
@@ -1796,12 +1922,15 @@
       <c r="G41" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H41" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>41</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1819,12 +1948,15 @@
       <c r="G42" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H42" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="B43" s="9"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="1" t="s">
         <v>13</v>
       </c>
@@ -1840,12 +1972,15 @@
       <c r="G43" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H43" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43</v>
       </c>
-      <c r="B44" s="9"/>
+      <c r="B44" s="10"/>
       <c r="C44" s="1" t="s">
         <v>14</v>
       </c>
@@ -1862,11 +1997,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>44</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="1" t="s">
         <v>15</v>
       </c>
@@ -1883,11 +2018,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="9"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="1" t="s">
         <v>16</v>
       </c>
@@ -1904,11 +2039,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>46</v>
       </c>
-      <c r="B47" s="9"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="1" t="s">
         <v>17</v>
       </c>
@@ -1925,11 +2060,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>47</v>
       </c>
-      <c r="B48" s="9"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="1" t="s">
         <v>36</v>
       </c>
@@ -1946,11 +2081,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>48</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="10"/>
       <c r="C49" s="1" t="s">
         <v>18</v>
       </c>
@@ -1966,12 +2101,15 @@
       <c r="G49" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H49" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="10"/>
       <c r="C50" s="1" t="s">
         <v>37</v>
       </c>
@@ -1987,12 +2125,15 @@
       <c r="G50" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H50" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>50</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="10"/>
       <c r="C51" s="1" t="s">
         <v>20</v>
       </c>
@@ -2008,8 +2149,11 @@
       <c r="G51" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H51" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="6">
         <v>51</v>
       </c>
@@ -2031,8 +2175,11 @@
       <c r="G52" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H52" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="6">
         <v>52</v>
       </c>
@@ -2054,9 +2201,13 @@
       <c r="G53" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="H53" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="H21:H24"/>
     <mergeCell ref="B42:B51"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B13"/>

</xml_diff>